<commit_message>
Avance tesina: EDA, clustering, estimación, ML y resultados
- config_figuras_tesina.py: estilos unificados para figuras
- Analisis_EDA.py / Analisis_cluster.py: ajustes y figuras EDA/cluster
- estimacion.py: flujo de estimación con relleno y clusters
- train_ml.py: entrenamiento KNN/XGBoost
- resultados_ml.py: análisis y gráficos de resultados ML
- data/processed: df_relleno, clusters actualizados, tabla resultados ML
- imagenes/: figuras EDA, cluster, estimación 3D y resultados ML

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/data/processed/df_rec_peso_pnd25.xlsx
+++ b/data/processed/df_rec_peso_pnd25.xlsx
@@ -746,7 +746,7 @@
         <v>10.7</v>
       </c>
       <c r="E18" t="n">
-        <v>-1.466507345781364</v>
+        <v>-1.466507345781363</v>
       </c>
     </row>
     <row r="19">
@@ -1222,7 +1222,7 @@
         <v>10.6</v>
       </c>
       <c r="E46" t="n">
-        <v>-1.496271989690777</v>
+        <v>-1.496271989690776</v>
       </c>
     </row>
     <row r="47">
@@ -1273,7 +1273,7 @@
         <v>23.5</v>
       </c>
       <c r="E49" t="n">
-        <v>1.016667270066598</v>
+        <v>1.016667270066597</v>
       </c>
     </row>
     <row r="50">
@@ -1511,7 +1511,7 @@
         <v>22.5</v>
       </c>
       <c r="E63" t="n">
-        <v>0.8682061057381122</v>
+        <v>0.8682061057381121</v>
       </c>
     </row>
     <row r="64">
@@ -1732,7 +1732,7 @@
         <v>22.8</v>
       </c>
       <c r="E76" t="n">
-        <v>0.9108728690353499</v>
+        <v>0.91087286903535</v>
       </c>
     </row>
     <row r="77">
@@ -2310,7 +2310,7 @@
         <v>24.35</v>
       </c>
       <c r="E110" t="n">
-        <v>1.099780121843102</v>
+        <v>1.099780121843101</v>
       </c>
     </row>
     <row r="111">
@@ -2395,7 +2395,7 @@
         <v>12.65</v>
       </c>
       <c r="E115" t="n">
-        <v>-0.8808881195869301</v>
+        <v>-0.8808881195869299</v>
       </c>
     </row>
     <row r="116">
@@ -2429,7 +2429,7 @@
         <v>25.09</v>
       </c>
       <c r="E117" t="n">
-        <v>1.174750424711061</v>
+        <v>1.174750424711062</v>
       </c>
     </row>
     <row r="118">
@@ -2582,7 +2582,7 @@
         <v>29.54</v>
       </c>
       <c r="E126" t="n">
-        <v>1.581998953410206</v>
+        <v>1.581998953410205</v>
       </c>
     </row>
     <row r="127">
@@ -2837,7 +2837,7 @@
         <v>11.21</v>
       </c>
       <c r="E141" t="n">
-        <v>-1.275302474602154</v>
+        <v>-1.275302474602153</v>
       </c>
     </row>
     <row r="142">
@@ -3041,7 +3041,7 @@
         <v>23.25</v>
       </c>
       <c r="E153" t="n">
-        <v>0.9836143965617343</v>
+        <v>0.9836143965617342</v>
       </c>
     </row>
     <row r="154">
@@ -3772,7 +3772,7 @@
         <v>22.78</v>
       </c>
       <c r="E196" t="n">
-        <v>0.9070697999135214</v>
+        <v>0.9070697999135215</v>
       </c>
     </row>
     <row r="197">
@@ -4282,7 +4282,7 @@
         <v>21.09</v>
       </c>
       <c r="E226" t="n">
-        <v>0.6920327496787795</v>
+        <v>0.6920327496787794</v>
       </c>
     </row>
     <row r="227">
@@ -4333,7 +4333,7 @@
         <v>13.33</v>
       </c>
       <c r="E229" t="n">
-        <v>-0.720438486837558</v>
+        <v>-0.7204384868375581</v>
       </c>
     </row>
     <row r="230">
@@ -5166,7 +5166,7 @@
         <v>12.58</v>
       </c>
       <c r="E278" t="n">
-        <v>-0.9108728690353499</v>
+        <v>-0.91087286903535</v>
       </c>
     </row>
     <row r="279">
@@ -5353,7 +5353,7 @@
         <v>11.95</v>
       </c>
       <c r="E289" t="n">
-        <v>-1.102204129666091</v>
+        <v>-1.102204129666092</v>
       </c>
     </row>
     <row r="290">
@@ -5676,7 +5676,7 @@
         <v>22.8</v>
       </c>
       <c r="E308" t="n">
-        <v>0.9108728690353499</v>
+        <v>0.91087286903535</v>
       </c>
     </row>
     <row r="309">
@@ -6645,7 +6645,7 @@
         <v>23.3</v>
       </c>
       <c r="E365" t="n">
-        <v>0.9931456094201364</v>
+        <v>0.9931456094201362</v>
       </c>
     </row>
     <row r="366">
@@ -6747,7 +6747,7 @@
         <v>22.9</v>
       </c>
       <c r="E371" t="n">
-        <v>0.9255717259908265</v>
+        <v>0.9255717259908262</v>
       </c>
     </row>
     <row r="372">
@@ -7155,7 +7155,7 @@
         <v>25.02</v>
       </c>
       <c r="E395" t="n">
-        <v>1.163759198525005</v>
+        <v>1.163759198525006</v>
       </c>
     </row>
     <row r="396">
@@ -7223,7 +7223,7 @@
         <v>36.46</v>
       </c>
       <c r="E399" t="n">
-        <v>2.03293829425014</v>
+        <v>2.032938294250141</v>
       </c>
     </row>
     <row r="400">
@@ -7240,7 +7240,7 @@
         <v>31.68</v>
       </c>
       <c r="E400" t="n">
-        <v>1.751488841246048</v>
+        <v>1.751488841246049</v>
       </c>
     </row>
     <row r="401">
@@ -7495,7 +7495,7 @@
         <v>24.55</v>
       </c>
       <c r="E415" t="n">
-        <v>1.127437725884891</v>
+        <v>1.127437725884892</v>
       </c>
     </row>
     <row r="416">
@@ -7563,7 +7563,7 @@
         <v>22.55</v>
       </c>
       <c r="E419" t="n">
-        <v>0.8759457518609561</v>
+        <v>0.8759457518609559</v>
       </c>
     </row>
     <row r="420">
@@ -7716,7 +7716,7 @@
         <v>22.61</v>
       </c>
       <c r="E428" t="n">
-        <v>0.8883093448377877</v>
+        <v>0.8883093448377878</v>
       </c>
     </row>
     <row r="429">
@@ -7971,7 +7971,7 @@
         <v>31.06</v>
       </c>
       <c r="E443" t="n">
-        <v>1.727223454437319</v>
+        <v>1.727223454437318</v>
       </c>
     </row>
     <row r="444">
@@ -8005,7 +8005,7 @@
         <v>22.94</v>
       </c>
       <c r="E445" t="n">
-        <v>0.9353231916648062</v>
+        <v>0.9353231916648064</v>
       </c>
     </row>
     <row r="446">
@@ -8056,7 +8056,7 @@
         <v>32.33</v>
       </c>
       <c r="E448" t="n">
-        <v>1.791764287378516</v>
+        <v>1.791764287378515</v>
       </c>
     </row>
     <row r="449">
@@ -8073,7 +8073,7 @@
         <v>28.18</v>
       </c>
       <c r="E449" t="n">
-        <v>1.48331976064457</v>
+        <v>1.483319760644569</v>
       </c>
     </row>
     <row r="450">
@@ -8124,7 +8124,7 @@
         <v>23.07</v>
       </c>
       <c r="E452" t="n">
-        <v>0.9629652676192322</v>
+        <v>0.9629652676192323</v>
       </c>
     </row>
     <row r="453">
@@ -8549,7 +8549,7 @@
         <v>25.39</v>
       </c>
       <c r="E477" t="n">
-        <v>1.204738646343397</v>
+        <v>1.204738646343398</v>
       </c>
     </row>
     <row r="478">
@@ -8906,7 +8906,7 @@
         <v>10.08</v>
       </c>
       <c r="E498" t="n">
-        <v>-1.674185775910646</v>
+        <v>-1.674185775910647</v>
       </c>
     </row>
     <row r="499">
@@ -9297,7 +9297,7 @@
         <v>26.53</v>
       </c>
       <c r="E521" t="n">
-        <v>1.321690549340496</v>
+        <v>1.321690549340497</v>
       </c>
     </row>
     <row r="522">
@@ -9416,7 +9416,7 @@
         <v>23.72</v>
       </c>
       <c r="E528" t="n">
-        <v>1.040530066337384</v>
+        <v>1.040530066337385</v>
       </c>
     </row>
     <row r="529">
@@ -9450,7 +9450,7 @@
         <v>22.76</v>
       </c>
       <c r="E530" t="n">
-        <v>0.9049849970908558</v>
+        <v>0.9049849970908557</v>
       </c>
     </row>
     <row r="531">
@@ -9501,7 +9501,7 @@
         <v>31.95</v>
       </c>
       <c r="E533" t="n">
-        <v>1.773469053704261</v>
+        <v>1.77346905370426</v>
       </c>
     </row>
     <row r="534">
@@ -9654,7 +9654,7 @@
         <v>11.21</v>
       </c>
       <c r="E542" t="n">
-        <v>-1.275302474602154</v>
+        <v>-1.275302474602153</v>
       </c>
     </row>
     <row r="543">
@@ -9688,7 +9688,7 @@
         <v>34.18</v>
       </c>
       <c r="E544" t="n">
-        <v>1.903945730478447</v>
+        <v>1.903945730478446</v>
       </c>
     </row>
     <row r="545">
@@ -9773,7 +9773,7 @@
         <v>39.17</v>
       </c>
       <c r="E549" t="n">
-        <v>2.226993604784915</v>
+        <v>2.226993604784916</v>
       </c>
     </row>
     <row r="550">
@@ -10113,7 +10113,7 @@
         <v>12.13</v>
       </c>
       <c r="E569" t="n">
-        <v>-1.033832286803353</v>
+        <v>-1.033832286803354</v>
       </c>
     </row>
     <row r="570">
@@ -10300,7 +10300,7 @@
         <v>24</v>
       </c>
       <c r="E580" t="n">
-        <v>1.070179963488353</v>
+        <v>1.070179963488352</v>
       </c>
     </row>
     <row r="581">
@@ -10334,7 +10334,7 @@
         <v>34.89</v>
       </c>
       <c r="E582" t="n">
-        <v>1.955802492185394</v>
+        <v>1.955802492185393</v>
       </c>
     </row>
     <row r="583">
@@ -10844,7 +10844,7 @@
         <v>25.57</v>
       </c>
       <c r="E612" t="n">
-        <v>1.222257725813505</v>
+        <v>1.222257725813506</v>
       </c>
     </row>
     <row r="613">
@@ -11014,7 +11014,7 @@
         <v>9.550000000000001</v>
       </c>
       <c r="E622" t="n">
-        <v>-1.855208512011559</v>
+        <v>-1.855208512011558</v>
       </c>
     </row>
     <row r="623">
@@ -11303,7 +11303,7 @@
         <v>12.65</v>
       </c>
       <c r="E639" t="n">
-        <v>-0.8808881195869301</v>
+        <v>-0.8808881195869299</v>
       </c>
     </row>
     <row r="640">
@@ -11371,7 +11371,7 @@
         <v>14.01</v>
       </c>
       <c r="E643" t="n">
-        <v>-0.5569266030950195</v>
+        <v>-0.5569266030950196</v>
       </c>
     </row>
     <row r="644">
@@ -11490,7 +11490,7 @@
         <v>14.01</v>
       </c>
       <c r="E650" t="n">
-        <v>-0.5569266030950195</v>
+        <v>-0.5569266030950196</v>
       </c>
     </row>
     <row r="651">
@@ -11507,7 +11507,7 @@
         <v>12.56</v>
       </c>
       <c r="E651" t="n">
-        <v>-0.9169462979277392</v>
+        <v>-0.9169462979277391</v>
       </c>
     </row>
     <row r="652">
@@ -11541,7 +11541,7 @@
         <v>10.08</v>
       </c>
       <c r="E653" t="n">
-        <v>-1.674185775910646</v>
+        <v>-1.674185775910647</v>
       </c>
     </row>
     <row r="654">
@@ -11966,7 +11966,7 @@
         <v>12.83</v>
       </c>
       <c r="E678" t="n">
-        <v>-0.8302341575863221</v>
+        <v>-0.8302341575863219</v>
       </c>
     </row>
     <row r="679">
@@ -11983,7 +11983,7 @@
         <v>12.77</v>
       </c>
       <c r="E679" t="n">
-        <v>-0.8446521467252646</v>
+        <v>-0.8446521467252647</v>
       </c>
     </row>
     <row r="680">
@@ -12408,7 +12408,7 @@
         <v>13.29</v>
       </c>
       <c r="E704" t="n">
-        <v>-0.7397372194138898</v>
+        <v>-0.73973721941389</v>
       </c>
     </row>
     <row r="705">
@@ -12510,7 +12510,7 @@
         <v>25.94</v>
       </c>
       <c r="E710" t="n">
-        <v>1.252840088418683</v>
+        <v>1.252840088418682</v>
       </c>
     </row>
     <row r="711">
@@ -12612,7 +12612,7 @@
         <v>22.85</v>
       </c>
       <c r="E716" t="n">
-        <v>0.9165019029489974</v>
+        <v>0.9165019029489971</v>
       </c>
     </row>
     <row r="717">
@@ -12850,7 +12850,7 @@
         <v>22.15</v>
       </c>
       <c r="E730" t="n">
-        <v>0.8156787628391502</v>
+        <v>0.8156787628391501</v>
       </c>
     </row>
     <row r="731">
@@ -12969,7 +12969,7 @@
         <v>23.21</v>
       </c>
       <c r="E737" t="n">
-        <v>0.9734327827708786</v>
+        <v>0.9734327827708785</v>
       </c>
     </row>
     <row r="738">
@@ -13071,7 +13071,7 @@
         <v>27.58</v>
       </c>
       <c r="E743" t="n">
-        <v>1.441897452229984</v>
+        <v>1.441897452229983</v>
       </c>
     </row>
     <row r="744">
@@ -13343,7 +13343,7 @@
         <v>23.86</v>
       </c>
       <c r="E759" t="n">
-        <v>1.058198970205179</v>
+        <v>1.058198970205178</v>
       </c>
     </row>
     <row r="760">
@@ -13360,7 +13360,7 @@
         <v>22.61</v>
       </c>
       <c r="E760" t="n">
-        <v>0.8883093448377877</v>
+        <v>0.8883093448377878</v>
       </c>
     </row>
     <row r="761">
@@ -13428,7 +13428,7 @@
         <v>13.25</v>
       </c>
       <c r="E764" t="n">
-        <v>-0.7442926555938575</v>
+        <v>-0.7442926555938577</v>
       </c>
     </row>
     <row r="765">
@@ -13462,7 +13462,7 @@
         <v>12.89</v>
       </c>
       <c r="E766" t="n">
-        <v>-0.8178049227354097</v>
+        <v>-0.8178049227354095</v>
       </c>
     </row>
     <row r="767">
@@ -13479,7 +13479,7 @@
         <v>13.53</v>
       </c>
       <c r="E767" t="n">
-        <v>-0.6590572416786885</v>
+        <v>-0.6590572416786886</v>
       </c>
     </row>
     <row r="768">
@@ -13785,7 +13785,7 @@
         <v>11.86</v>
       </c>
       <c r="E785" t="n">
-        <v>-1.116368890290762</v>
+        <v>-1.116368890290763</v>
       </c>
     </row>
     <row r="786">
@@ -13802,7 +13802,7 @@
         <v>14.01</v>
       </c>
       <c r="E786" t="n">
-        <v>-0.5569266030950195</v>
+        <v>-0.5569266030950196</v>
       </c>
     </row>
     <row r="787">
@@ -13955,7 +13955,7 @@
         <v>25.85</v>
       </c>
       <c r="E795" t="n">
-        <v>1.245510272321044</v>
+        <v>1.245510272321043</v>
       </c>
     </row>
     <row r="796">
@@ -13989,7 +13989,7 @@
         <v>12.49</v>
       </c>
       <c r="E797" t="n">
-        <v>-0.9377977680303106</v>
+        <v>-0.9377977680303105</v>
       </c>
     </row>
     <row r="798">
@@ -14040,7 +14040,7 @@
         <v>12.49</v>
       </c>
       <c r="E800" t="n">
-        <v>-0.9377977680303106</v>
+        <v>-0.9377977680303105</v>
       </c>
     </row>
     <row r="801">
@@ -14108,7 +14108,7 @@
         <v>20</v>
       </c>
       <c r="E804" t="n">
-        <v>0.5395988872028697</v>
+        <v>0.5395988872028699</v>
       </c>
     </row>
     <row r="805">
@@ -14125,7 +14125,7 @@
         <v>12.62</v>
       </c>
       <c r="E805" t="n">
-        <v>-0.8888400117499844</v>
+        <v>-0.8888400117499843</v>
       </c>
     </row>
     <row r="806">
@@ -14142,7 +14142,7 @@
         <v>12.42</v>
       </c>
       <c r="E806" t="n">
-        <v>-0.9608536026483906</v>
+        <v>-0.9608536026483905</v>
       </c>
     </row>
     <row r="807">
@@ -14295,7 +14295,7 @@
         <v>32.82</v>
       </c>
       <c r="E815" t="n">
-        <v>1.813721856298946</v>
+        <v>1.813721856298947</v>
       </c>
     </row>
     <row r="816">
@@ -15315,7 +15315,7 @@
         <v>23.05</v>
       </c>
       <c r="E875" t="n">
-        <v>0.9598238702141551</v>
+        <v>0.9598238702141553</v>
       </c>
     </row>
     <row r="876">
@@ -16080,7 +16080,7 @@
         <v>14.54</v>
       </c>
       <c r="E920" t="n">
-        <v>-0.4388180848338032</v>
+        <v>-0.4388180848338031</v>
       </c>
     </row>
     <row r="921">
@@ -16250,7 +16250,7 @@
         <v>20.37</v>
       </c>
       <c r="E930" t="n">
-        <v>0.5900692211395775</v>
+        <v>0.5900692211395774</v>
       </c>
     </row>
     <row r="931">
@@ -16318,7 +16318,7 @@
         <v>12.41</v>
       </c>
       <c r="E934" t="n">
-        <v>-0.9636475233995441</v>
+        <v>-0.9636475233995438</v>
       </c>
     </row>
     <row r="935">
@@ -16437,7 +16437,7 @@
         <v>12.83</v>
       </c>
       <c r="E941" t="n">
-        <v>-0.8302341575863221</v>
+        <v>-0.8302341575863219</v>
       </c>
     </row>
     <row r="942">
@@ -16964,7 +16964,7 @@
         <v>23.42</v>
       </c>
       <c r="E972" t="n">
-        <v>1.004362137503493</v>
+        <v>1.004362137503492</v>
       </c>
     </row>
     <row r="973">
@@ -17083,7 +17083,7 @@
         <v>12.77</v>
       </c>
       <c r="E979" t="n">
-        <v>-0.8446521467252646</v>
+        <v>-0.8446521467252647</v>
       </c>
     </row>
     <row r="980">
@@ -17321,7 +17321,7 @@
         <v>10.92</v>
       </c>
       <c r="E993" t="n">
-        <v>-1.419549387150268</v>
+        <v>-1.419549387150267</v>
       </c>
     </row>
     <row r="994">
@@ -17389,7 +17389,7 @@
         <v>12.58</v>
       </c>
       <c r="E997" t="n">
-        <v>-0.9108728690353499</v>
+        <v>-0.91087286903535</v>
       </c>
     </row>
     <row r="998">
@@ -17406,7 +17406,7 @@
         <v>13.29</v>
       </c>
       <c r="E998" t="n">
-        <v>-0.7397372194138898</v>
+        <v>-0.73973721941389</v>
       </c>
     </row>
     <row r="999">
@@ -17474,7 +17474,7 @@
         <v>12.55</v>
       </c>
       <c r="E1002" t="n">
-        <v>-0.9193840350404709</v>
+        <v>-0.9193840350404711</v>
       </c>
     </row>
     <row r="1003">
@@ -17848,7 +17848,7 @@
         <v>12.07</v>
       </c>
       <c r="E1024" t="n">
-        <v>-1.054438857783394</v>
+        <v>-1.054438857783395</v>
       </c>
     </row>
     <row r="1025">
@@ -18256,7 +18256,7 @@
         <v>22.66</v>
       </c>
       <c r="E1048" t="n">
-        <v>0.894577291374814</v>
+        <v>0.8945772913748138</v>
       </c>
     </row>
     <row r="1049">
@@ -18307,7 +18307,7 @@
         <v>12.63</v>
       </c>
       <c r="E1051" t="n">
-        <v>-0.8864505912695492</v>
+        <v>-0.8864505912695493</v>
       </c>
     </row>
     <row r="1052">
@@ -18324,7 +18324,7 @@
         <v>12.48</v>
       </c>
       <c r="E1052" t="n">
-        <v>-0.9408879068214815</v>
+        <v>-0.9408879068214813</v>
       </c>
     </row>
     <row r="1053">
@@ -18375,7 +18375,7 @@
         <v>11.86</v>
       </c>
       <c r="E1055" t="n">
-        <v>-1.116368890290762</v>
+        <v>-1.116368890290763</v>
       </c>
     </row>
     <row r="1056">
@@ -18494,7 +18494,7 @@
         <v>13.29</v>
       </c>
       <c r="E1062" t="n">
-        <v>-0.7397372194138898</v>
+        <v>-0.73973721941389</v>
       </c>
     </row>
     <row r="1063">
@@ -19174,7 +19174,7 @@
         <v>10.8</v>
       </c>
       <c r="E1102" t="n">
-        <v>-1.445573326263457</v>
+        <v>-1.445573326263456</v>
       </c>
     </row>
     <row r="1103">
@@ -19446,7 +19446,7 @@
         <v>10.24</v>
       </c>
       <c r="E1118" t="n">
-        <v>-1.57095689421494</v>
+        <v>-1.570956894214939</v>
       </c>
     </row>
     <row r="1119">
@@ -19803,7 +19803,7 @@
         <v>9.74</v>
       </c>
       <c r="E1139" t="n">
-        <v>-1.794270820978285</v>
+        <v>-1.794270820978284</v>
       </c>
     </row>
     <row r="1140">
@@ -19990,7 +19990,7 @@
         <v>13.32</v>
       </c>
       <c r="E1150" t="n">
-        <v>-0.7230720375879418</v>
+        <v>-0.7230720375879416</v>
       </c>
     </row>
     <row r="1151">
@@ -20211,7 +20211,7 @@
         <v>10.54</v>
       </c>
       <c r="E1163" t="n">
-        <v>-1.509488119671934</v>
+        <v>-1.509488119671935</v>
       </c>
     </row>
     <row r="1164">
@@ -20398,7 +20398,7 @@
         <v>12.59</v>
       </c>
       <c r="E1174" t="n">
-        <v>-0.9070613893606347</v>
+        <v>-0.9070613893606345</v>
       </c>
     </row>
     <row r="1175">
@@ -21163,7 +21163,7 @@
         <v>9.5</v>
       </c>
       <c r="E1219" t="n">
-        <v>-1.871188480525936</v>
+        <v>-1.871188480525935</v>
       </c>
     </row>
     <row r="1220">
@@ -21418,7 +21418,7 @@
         <v>12.31</v>
       </c>
       <c r="E1234" t="n">
-        <v>-0.9975733229149144</v>
+        <v>-0.9975733229149146</v>
       </c>
     </row>
     <row r="1235">

</xml_diff>